<commit_message>
Fix mistake in edited-species7.csv, was miss a duplicate row
</commit_message>
<xml_diff>
--- a/data/raw/01b_edited-species8_location-dependent-final-fix.xlsx
+++ b/data/raw/01b_edited-species8_location-dependent-final-fix.xlsx
@@ -3846,8 +3846,8 @@
   <dimension ref="A1:H322"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J318" sqref="J318"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>